<commit_message>
added loop for prediction draws
</commit_message>
<xml_diff>
--- a/aggregate_calibration_output.xlsx
+++ b/aggregate_calibration_output.xlsx
@@ -464,61 +464,61 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>10801997.70220176</v>
+        <v>10801999.03673311</v>
       </c>
       <c r="C2">
-        <v>2398747.128764417</v>
+        <v>2414466.439874003</v>
       </c>
       <c r="D2">
-        <v>27947563.08115542</v>
+        <v>28111992.96818429</v>
       </c>
       <c r="E2">
-        <v>1179282.562991061</v>
+        <v>1189901.79008772</v>
       </c>
       <c r="F2">
-        <v>9614104.594186693</v>
+        <v>9486554.436699318</v>
       </c>
       <c r="G2">
-        <v>1822547.333998816</v>
+        <v>1806289.812291691</v>
       </c>
       <c r="H2">
-        <v>2208122.123670813</v>
+        <v>2157083.447618817</v>
       </c>
       <c r="I2">
-        <v>10801997.70220176</v>
+        <v>10801999.03673311</v>
       </c>
       <c r="J2">
-        <v>45553002</v>
+        <v>45425814</v>
       </c>
       <c r="K2">
         <v>123</v>
       </c>
       <c r="L2">
-        <v>30346310.20991984</v>
+        <v>30526459.40805829</v>
       </c>
       <c r="M2">
-        <v>10793387.15717775</v>
+        <v>10676456.22678704</v>
       </c>
       <c r="N2">
-        <v>4030669.457669629</v>
+        <v>3963373.259910508</v>
       </c>
       <c r="O2">
-        <v>45702.16184636338</v>
+        <v>38154.79029512414</v>
       </c>
       <c r="P2">
-        <v>213835.2085858153</v>
+        <v>198626.9279718958</v>
       </c>
       <c r="Q2">
-        <v>259537.3704321787</v>
+        <v>236781.71826702</v>
       </c>
       <c r="R2">
-        <v>372.3568862079573</v>
+        <v>361.6488484323222</v>
       </c>
       <c r="S2">
-        <v>110489.8498057205</v>
+        <v>112369.8360000918</v>
       </c>
       <c r="T2">
-        <v>110862.2066919285</v>
+        <v>112731.4848485241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjust cdf star, test runs
</commit_message>
<xml_diff>
--- a/aggregate_calibration_output.xlsx
+++ b/aggregate_calibration_output.xlsx
@@ -464,61 +464,61 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>10801997.16629423</v>
+        <v>10775351.92785637</v>
       </c>
       <c r="C2">
-        <v>2390776.998132432</v>
+        <v>2429237.833225261</v>
       </c>
       <c r="D2">
-        <v>27877165.35240201</v>
+        <v>28250397.67641928</v>
       </c>
       <c r="E2">
-        <v>1156766.700284801</v>
+        <v>1176877.84930499</v>
       </c>
       <c r="F2">
-        <v>9423542.157534683</v>
+        <v>9397656.956019122</v>
       </c>
       <c r="G2">
-        <v>1844372.631350089</v>
+        <v>1848931.834534268</v>
       </c>
       <c r="H2">
-        <v>2190022.0637029</v>
+        <v>2100844.41724581</v>
       </c>
       <c r="I2">
-        <v>10801997.16629423</v>
+        <v>10775351.92785637</v>
       </c>
       <c r="J2">
-        <v>44939105</v>
+        <v>44940247</v>
       </c>
       <c r="K2">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="L2">
-        <v>30267942.35053444</v>
+        <v>30679635.50964454</v>
       </c>
       <c r="M2">
-        <v>10580308.85781949</v>
+        <v>10574534.80532411</v>
       </c>
       <c r="N2">
-        <v>4034394.695052989</v>
+        <v>3949776.251780078</v>
       </c>
       <c r="O2">
-        <v>39494.24410204964</v>
+        <v>41293.57878157049</v>
       </c>
       <c r="P2">
-        <v>205722.923454306</v>
+        <v>206574.1005918898</v>
       </c>
       <c r="Q2">
-        <v>245217.1675563557</v>
+        <v>247867.6793734603</v>
       </c>
       <c r="R2">
-        <v>363.3855534273681</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>111510.0611290252</v>
+        <v>109448.5612180983</v>
       </c>
       <c r="T2">
-        <v>111873.4466824526</v>
+        <v>109448.5612180983</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjusted projected harvest per trip, tested model
</commit_message>
<xml_diff>
--- a/aggregate_calibration_output.xlsx
+++ b/aggregate_calibration_output.xlsx
@@ -464,61 +464,61 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>10775354.73282147</v>
+        <v>10775351.19246996</v>
       </c>
       <c r="C2">
-        <v>2355658.058386934</v>
+        <v>2333037.159199236</v>
       </c>
       <c r="D2">
-        <v>26719498.71858908</v>
+        <v>26681052.94840628</v>
       </c>
       <c r="E2">
-        <v>1160060.286615036</v>
+        <v>1138278.49584407</v>
       </c>
       <c r="F2">
-        <v>8089757.170563366</v>
+        <v>7896047.847144105</v>
       </c>
       <c r="G2">
-        <v>1853669.720710634</v>
+        <v>1842394.1173711</v>
       </c>
       <c r="H2">
-        <v>2141944.933309767</v>
+        <v>2144817.388797354</v>
       </c>
       <c r="I2">
-        <v>10775354.73282147</v>
+        <v>10775351.19246996</v>
       </c>
       <c r="J2">
-        <v>45316349</v>
+        <v>45373051</v>
       </c>
       <c r="K2">
         <v>112</v>
       </c>
       <c r="L2">
-        <v>29075156.77697601</v>
+        <v>29014090.10760552</v>
       </c>
       <c r="M2">
-        <v>9249817.457178403</v>
+        <v>9034326.342988174</v>
       </c>
       <c r="N2">
-        <v>3995614.654020401</v>
+        <v>3987211.506168454</v>
       </c>
       <c r="O2">
-        <v>43009.07809124866</v>
+        <v>42661.91286283184</v>
       </c>
       <c r="P2">
-        <v>202817.3567267472</v>
+        <v>203894.3726773379</v>
       </c>
       <c r="Q2">
-        <v>245826.4348179959</v>
+        <v>246556.2855401697</v>
       </c>
       <c r="R2">
         <v>0</v>
       </c>
       <c r="S2">
-        <v>105370.6424610647</v>
+        <v>104322.4875383274</v>
       </c>
       <c r="T2">
-        <v>105370.6424610647</v>
+        <v>104322.4875383274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new selectivity and test runs
</commit_message>
<xml_diff>
--- a/aggregate_calibration_output.xlsx
+++ b/aggregate_calibration_output.xlsx
@@ -464,61 +464,61 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>10801998.67284607</v>
+        <v>10801997.17295967</v>
       </c>
       <c r="C2">
-        <v>2390706.027224486</v>
+        <v>2374074.297282989</v>
       </c>
       <c r="D2">
-        <v>26646187.82939581</v>
+        <v>26378827.89743374</v>
       </c>
       <c r="E2">
-        <v>1176717.865767175</v>
+        <v>1185682.38352715</v>
       </c>
       <c r="F2">
-        <v>8317910.046689478</v>
+        <v>8439986.56294816</v>
       </c>
       <c r="G2">
-        <v>1833488.527353045</v>
+        <v>1828197.521994759</v>
       </c>
       <c r="H2">
-        <v>2135770.015141096</v>
+        <v>2104549.666711418</v>
       </c>
       <c r="I2">
-        <v>10801998.67284607</v>
+        <v>10801997.17295967</v>
       </c>
       <c r="J2">
-        <v>45486215</v>
+        <v>45512584</v>
       </c>
       <c r="K2">
         <v>123</v>
       </c>
       <c r="L2">
-        <v>29036893.8566203</v>
+        <v>28752902.19471672</v>
       </c>
       <c r="M2">
-        <v>9494627.912456652</v>
+        <v>9625668.94647531</v>
       </c>
       <c r="N2">
-        <v>3969258.542494141</v>
+        <v>3932747.188706177</v>
       </c>
       <c r="O2">
-        <v>42058.40563440622</v>
+        <v>45117.65828076528</v>
       </c>
       <c r="P2">
-        <v>207175.8522433573</v>
+        <v>206824.7031532861</v>
       </c>
       <c r="Q2">
-        <v>249234.2578777635</v>
+        <v>251942.3614340514</v>
       </c>
       <c r="R2">
         <v>0</v>
       </c>
       <c r="S2">
-        <v>111171.2040422165</v>
+        <v>116051.4494870003</v>
       </c>
       <c r="T2">
-        <v>111171.2040422165</v>
+        <v>116051.4494870003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjustments and test runs
</commit_message>
<xml_diff>
--- a/aggregate_calibration_output.xlsx
+++ b/aggregate_calibration_output.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -430,30 +430,35 @@
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
+          <t>Group.1</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
           <t>tot_keep_wf</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>tot_rel_wf</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>tot_wf_cat</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>tot_keep_rd</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>tot_rel_rd</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>tot_rd_cat</t>
         </is>
@@ -464,61 +469,64 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>10801998.75377954</v>
+        <v>10801998.33475939</v>
       </c>
       <c r="C2">
-        <v>2355449.873675503</v>
+        <v>2372282.164526457</v>
       </c>
       <c r="D2">
-        <v>26420149.15756752</v>
+        <v>26557345.39449133</v>
       </c>
       <c r="E2">
-        <v>1170335.67459554</v>
+        <v>1152364.165444766</v>
       </c>
       <c r="F2">
-        <v>8304634.029621447</v>
+        <v>8085423.201825836</v>
       </c>
       <c r="G2">
-        <v>1803776.560677967</v>
+        <v>1840377.530403443</v>
       </c>
       <c r="H2">
-        <v>2142420.406991235</v>
+        <v>2146872.416877256</v>
       </c>
       <c r="I2">
-        <v>10801998.75377954</v>
+        <v>10801998.33475939</v>
       </c>
       <c r="J2">
-        <v>45566403</v>
+        <v>45590812</v>
       </c>
       <c r="K2">
         <v>123</v>
       </c>
       <c r="L2">
-        <v>28775599.03124302</v>
+        <v>28929627.55901779</v>
       </c>
       <c r="M2">
-        <v>9474969.704216985</v>
+        <v>9237787.367270602</v>
       </c>
       <c r="N2">
-        <v>3946196.967669202</v>
+        <v>3987249.947280699</v>
       </c>
       <c r="O2">
-        <v>47460.68873488131</v>
+        <v>6750225000</v>
       </c>
       <c r="P2">
-        <v>201529.7336367138</v>
+        <v>42014.73273041348</v>
       </c>
       <c r="Q2">
-        <v>248990.4223715951</v>
+        <v>205086.7601341055</v>
       </c>
       <c r="R2">
+        <v>247101.492864519</v>
+      </c>
+      <c r="S2">
         <v>0</v>
       </c>
-      <c r="S2">
-        <v>112434.7499023176</v>
-      </c>
       <c r="T2">
-        <v>112434.7499023176</v>
+        <v>109763.5155576515</v>
+      </c>
+      <c r="U2">
+        <v>109763.5155576515</v>
       </c>
     </row>
   </sheetData>

</xml_diff>